<commit_message>
Add get email credentials
</commit_message>
<xml_diff>
--- a/CV Break In.xlsx
+++ b/CV Break In.xlsx
@@ -99,7 +99,7 @@
     <t>rpa</t>
   </si>
   <si>
-    <t>it</t>
+    <t xml:space="preserve"> it </t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Add get email credentials"
This reverts commit 8a04126f951594b2fce61a55f81f70240866cacd.
</commit_message>
<xml_diff>
--- a/CV Break In.xlsx
+++ b/CV Break In.xlsx
@@ -99,7 +99,7 @@
     <t>rpa</t>
   </si>
   <si>
-    <t xml:space="preserve"> it </t>
+    <t>it</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refine style and format
</commit_message>
<xml_diff>
--- a/CV Break In.xlsx
+++ b/CV Break In.xlsx
@@ -99,7 +99,7 @@
     <t>rpa</t>
   </si>
   <si>
-    <t>it</t>
+    <t xml:space="preserve"> it </t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>